<commit_message>
I updated the data and publishing work in the proposal and the sub page.
</commit_message>
<xml_diff>
--- a/02_2018portfolio/00_plan/project_contents_jschoi.xlsx
+++ b/02_2018portfolio/00_plan/project_contents_jschoi.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\4. connect_git\PORTFOLIO\02_2018portfolio\00_plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4. connect_git\PORTFOLIO\02_2018portfolio\00_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -130,20 +130,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>내부망인 환경방사능실험공정관리시스템의
-관리자페이지와 사용자페이지 전체 퍼블리싱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>내부망인 LX도로대장 정보시스템 로그인 페이지 디자인 및 퍼블리싱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>내부망인 통합고객관리시스템 페이지 중 대표페이지 퍼블리싱 및 아시아문화전당 로그인후 예매시 나오는 결제페이지 퍼블리싱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.05 ~ 2017.07</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -255,13 +246,22 @@
   <si>
     <t>관리자페이지는 페이지별로 링크
 연결하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.05 ~ 2017.07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내부망인 환경방사능실험공정관리시스템의
+관리자페이지와 사용자페이지 전체 퍼블리싱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -680,7 +680,7 @@
         <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
@@ -694,22 +694,22 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -718,22 +718,22 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="H3" s="1">
         <v>2017.12</v>
@@ -744,22 +744,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H4" s="1">
         <v>2017.12</v>
@@ -770,25 +770,25 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -796,22 +796,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1">
         <v>2017.07</v>
@@ -831,13 +831,13 @@
         <v>25</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="H7" s="1">
         <v>2017.05</v>
@@ -860,7 +860,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>23</v>
@@ -883,7 +883,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>15</v>
@@ -909,7 +909,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>6</v>

</xml_diff>